<commit_message>
Change in Sate Realtion Excel File
</commit_message>
<xml_diff>
--- a/StateList.xlsx
+++ b/StateList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/4th Sem/DAA/M-Colouring-Problem/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51053797-003A-B84B-9155-7DC3A7CEE00C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA8363B-2106-AB49-A468-F2C30E454A6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13000" yWindow="0" windowWidth="12600" windowHeight="16000" xr2:uid="{B8DDEBB0-1D1A-CF4B-B83F-6E8BE02E01C9}"/>
+    <workbookView xWindow="13000" yWindow="460" windowWidth="12600" windowHeight="14480" xr2:uid="{B8DDEBB0-1D1A-CF4B-B83F-6E8BE02E01C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t>Name of the state</t>
   </si>
@@ -141,33 +141,18 @@
     <t>West Bengal</t>
   </si>
   <si>
-    <t>2,3</t>
-  </si>
-  <si>
-    <t>1,3,5,6</t>
-  </si>
-  <si>
     <t>1,2,4,6,8</t>
   </si>
   <si>
     <t>3,6</t>
   </si>
   <si>
-    <t>2,9</t>
-  </si>
-  <si>
-    <t>2,3,7,8,9</t>
-  </si>
-  <si>
     <t>6,9</t>
   </si>
   <si>
     <t>3,6,9,23,24</t>
   </si>
   <si>
-    <t>2,5,6,7,8,10,20,22,23</t>
-  </si>
-  <si>
     <t>9,19,20</t>
   </si>
   <si>
@@ -192,49 +177,70 @@
     <t>10,11,18,20,21</t>
   </si>
   <si>
-    <t>9,23,22,21,19,10</t>
-  </si>
-  <si>
     <t>19,20,22,28</t>
   </si>
   <si>
-    <t>20,9,23,27,36,37,21</t>
-  </si>
-  <si>
-    <t>24,8,9,22</t>
-  </si>
-  <si>
     <t>24,27</t>
   </si>
   <si>
-    <t>8,23,27,25,26</t>
-  </si>
-  <si>
-    <t>24,26,23,22,36,30,29</t>
-  </si>
-  <si>
-    <t>21,22,36,29,33,34</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>30,27,36,28,33,32</t>
-  </si>
-  <si>
     <t>27,29</t>
   </si>
   <si>
     <t>29,33,34</t>
   </si>
   <si>
-    <t>32,29,28,34</t>
-  </si>
-  <si>
-    <t>33,32,28</t>
-  </si>
-  <si>
-    <t>27,22,28,29</t>
+    <t>2,3,37</t>
+  </si>
+  <si>
+    <t>1,3,5,6,37</t>
+  </si>
+  <si>
+    <t>5,6,7,8,10,20,22,23</t>
+  </si>
+  <si>
+    <t>9,10,19,21,22,23</t>
+  </si>
+  <si>
+    <t>8,23,25,26,27</t>
+  </si>
+  <si>
+    <t>22,23,24,26,29,30,36</t>
+  </si>
+  <si>
+    <t>8,9,22,24,27</t>
+  </si>
+  <si>
+    <t>21,22,29,33,34,36</t>
+  </si>
+  <si>
+    <t>9,20,21,23,27,28,36</t>
+  </si>
+  <si>
+    <t>27,28,30,32,33,36</t>
+  </si>
+  <si>
+    <t>28,29,32,34</t>
+  </si>
+  <si>
+    <t>28,32,33</t>
+  </si>
+  <si>
+    <t>22,27,28,29</t>
+  </si>
+  <si>
+    <t>Ladakh</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>2,6,9</t>
+  </si>
+  <si>
+    <t>2,3,4,5,7,8,9</t>
   </si>
 </sst>
 </file>
@@ -602,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E917DD5-DF2D-E74B-B21A-1CA67D73E309}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="119" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -629,7 +635,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18">
@@ -640,7 +646,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18">
@@ -651,7 +657,7 @@
         <v>29</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18">
@@ -662,7 +668,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18">
@@ -673,7 +679,7 @@
         <v>36</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18">
@@ -684,7 +690,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18">
@@ -695,7 +701,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18">
@@ -706,7 +712,7 @@
         <v>30</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18">
@@ -717,7 +723,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18">
@@ -728,7 +734,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18">
@@ -750,7 +756,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18">
@@ -761,7 +767,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18">
@@ -772,7 +778,7 @@
         <v>23</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18">
@@ -783,7 +789,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="18">
@@ -794,7 +800,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="18">
@@ -816,7 +822,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="18">
@@ -827,7 +833,7 @@
         <v>37</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="18">
@@ -838,7 +844,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="18">
@@ -849,7 +855,7 @@
         <v>27</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="18">
@@ -860,7 +866,7 @@
         <v>8</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="18">
@@ -871,7 +877,7 @@
         <v>21</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="18">
@@ -882,7 +888,7 @@
         <v>13</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="18">
@@ -904,7 +910,7 @@
         <v>9</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18">
@@ -915,7 +921,7 @@
         <v>22</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="18">
@@ -948,7 +954,7 @@
         <v>12</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="18">
@@ -970,7 +976,7 @@
         <v>19</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="18">
@@ -981,7 +987,7 @@
         <v>32</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="18">
@@ -992,7 +998,7 @@
         <v>28</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="18">
@@ -1014,23 +1020,26 @@
         <v>33</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="18">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="18">
-      <c r="A38" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="18">
       <c r="A39" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>